<commit_message>
added 18 to 21
</commit_message>
<xml_diff>
--- a/pandas_study/data/summary.xlsx
+++ b/pandas_study/data/summary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18468" windowHeight="9420" tabRatio="735" firstSheet="3" activeTab="10"/>
+    <workbookView windowWidth="18468" windowHeight="9420" tabRatio="735" firstSheet="7" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="pie" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,10 @@
     <sheet name="student" sheetId="9" r:id="rId9"/>
     <sheet name="score" sheetId="10" r:id="rId10"/>
     <sheet name="checkout" sheetId="11" r:id="rId11"/>
+    <sheet name="split name" sheetId="12" r:id="rId12"/>
+    <sheet name="average" sheetId="13" r:id="rId13"/>
+    <sheet name="duplicated" sheetId="14" r:id="rId14"/>
+    <sheet name="transform" sheetId="15" r:id="rId15"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">filter!$A$1:$D$21</definedName>
@@ -60,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="158">
   <si>
     <t>Field</t>
   </si>
@@ -431,6 +435,114 @@
   </si>
   <si>
     <t>student_20</t>
+  </si>
+  <si>
+    <t>Full</t>
+  </si>
+  <si>
+    <t>Syed</t>
+  </si>
+  <si>
+    <t>Abbas</t>
+  </si>
+  <si>
+    <t>Catherine</t>
+  </si>
+  <si>
+    <t>Abel</t>
+  </si>
+  <si>
+    <t>Kim</t>
+  </si>
+  <si>
+    <t>Aber</t>
+  </si>
+  <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>Abo</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Adams</t>
+  </si>
+  <si>
+    <t>Angle</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>Test_1</t>
+  </si>
+  <si>
+    <t>Test_2</t>
+  </si>
+  <si>
+    <t>Test3</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>student_002</t>
+  </si>
+  <si>
+    <t>student_004</t>
+  </si>
+  <si>
+    <t>student_006</t>
+  </si>
+  <si>
+    <t>student_008</t>
+  </si>
+  <si>
+    <t>student_010</t>
+  </si>
+  <si>
+    <t>summary</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Active User</t>
+  </si>
+  <si>
+    <t>Page View</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>Apr</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>Jul</t>
+  </si>
+  <si>
+    <t>Aug</t>
+  </si>
+  <si>
+    <t>Sep</t>
   </si>
 </sst>
 </file>
@@ -440,8 +552,8 @@
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -460,12 +572,35 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
@@ -474,10 +609,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="等线"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -489,8 +624,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -512,52 +685,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF7F7F7F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -573,31 +709,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -614,12 +726,18 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -629,19 +747,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -653,7 +777,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -665,31 +843,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -701,43 +855,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -749,19 +867,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -779,13 +891,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -797,19 +903,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -823,17 +941,52 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -843,15 +996,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -873,17 +1017,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -891,31 +1024,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -926,10 +1044,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -938,142 +1056,144 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -7965,32 +8085,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4">
+      <c r="B1" s="6">
         <v>2016</v>
       </c>
-      <c r="C1" s="4">
+      <c r="C1" s="6">
         <v>2017</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="5">
         <v>216932</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="5">
         <v>230711</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="5">
         <v>200312</v>
       </c>
       <c r="C3">
@@ -7998,65 +8118,65 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="5">
         <v>141651</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="5">
         <v>167180</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="5">
         <v>81318</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="5">
         <v>87577</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="5">
         <v>81304</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="5">
         <v>83046</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="5">
         <v>75385</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="5">
         <v>76838</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="5">
         <v>59736</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="5">
         <v>61506</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="5">
         <v>40877</v>
       </c>
       <c r="C9">
@@ -8064,73 +8184,73 @@
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="5">
         <v>21160</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="5">
         <v>21913</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="5">
         <v>26675</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="5">
         <v>21131</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="5">
         <v>19483</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="5">
         <v>17993</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="5">
         <v>17664</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="5">
         <v>17561</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="5">
         <v>15077</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="5">
         <v>15306</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="5">
         <v>12318</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="5">
         <v>12602</v>
       </c>
     </row>
     <row r="20" ht="41.4" spans="5:5">
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="9" t="s">
         <v>15</v>
       </c>
     </row>
@@ -8159,170 +8279,170 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="2">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="3">
         <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="2">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="3">
         <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="2">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="3">
         <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="2">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="3">
         <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="2">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="3">
         <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="2">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="3">
         <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="2">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="3">
         <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="2">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="3">
         <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="2">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="3">
         <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="2">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="3">
         <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="2">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="3">
         <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="2">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="3">
         <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="2">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="3">
         <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="2">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="3">
         <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="2">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="3">
         <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="2">
+      <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="3">
         <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="2">
+      <c r="A18" s="3">
         <v>17</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="3">
         <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="2">
+      <c r="A19" s="3">
         <v>18</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="3">
         <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="2">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="3">
         <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="2">
+      <c r="A21" s="3">
         <v>20</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="3">
         <v>93</v>
       </c>
     </row>
@@ -8337,7 +8457,7 @@
   <sheetPr/>
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -8347,233 +8467,233 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="1">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="3">
         <v>-40</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="1">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="3">
         <v>-30</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="1">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="3">
         <v>-20</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="1">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="3">
         <v>-10</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="1">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="1">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="3">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="1">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="3">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="1">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="3">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="1">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="3">
         <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="1">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="3">
         <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="1">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="3">
         <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="1">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="3">
         <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="1">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="3">
         <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="1">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="3">
         <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="1">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="3">
         <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="1">
+      <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="3">
         <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="1">
+      <c r="A18" s="3">
         <v>17</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="3">
         <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="1">
+      <c r="A19" s="3">
         <v>18</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="3">
         <v>130</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="1">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="3">
         <v>140</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="1">
+      <c r="A21" s="3">
         <v>20</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="3">
         <v>150</v>
       </c>
     </row>
@@ -8589,6 +8709,902 @@
   <ignoredErrors>
     <ignoredError sqref="C1" listDataValidation="1"/>
   </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="13.8" outlineLevelCol="2"/>
+  <cols>
+    <col min="2" max="2" width="17.7777777777778" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="13.8" outlineLevelCol="6"/>
+  <cols>
+    <col min="2" max="2" width="15.5555555555556" customWidth="1"/>
+    <col min="7" max="7" width="12.8888888888889"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="1">
+        <v>55</v>
+      </c>
+      <c r="D2" s="1">
+        <v>68</v>
+      </c>
+      <c r="E2" s="1">
+        <v>90</v>
+      </c>
+      <c r="F2" s="1">
+        <f t="shared" ref="F2:F11" si="0">SUM(C2:E2)</f>
+        <v>213</v>
+      </c>
+      <c r="G2" s="1">
+        <f t="shared" ref="G2:G11" si="1">AVERAGE(C2:E2)</f>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C3" s="1">
+        <v>56</v>
+      </c>
+      <c r="D3" s="1">
+        <v>69</v>
+      </c>
+      <c r="E3" s="1">
+        <v>91</v>
+      </c>
+      <c r="F3" s="1">
+        <f t="shared" si="0"/>
+        <v>216</v>
+      </c>
+      <c r="G3" s="1">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="1">
+        <v>57</v>
+      </c>
+      <c r="D4" s="1">
+        <v>70</v>
+      </c>
+      <c r="E4" s="1">
+        <v>92</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" si="0"/>
+        <v>219</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="1">
+        <v>58</v>
+      </c>
+      <c r="D5" s="1">
+        <v>71</v>
+      </c>
+      <c r="E5" s="1">
+        <v>77</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="0"/>
+        <v>206</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="1"/>
+        <v>68.6666666666667</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" s="1">
+        <v>80</v>
+      </c>
+      <c r="D6" s="1">
+        <v>72</v>
+      </c>
+      <c r="E6" s="1">
+        <v>78</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="0"/>
+        <v>230</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="1"/>
+        <v>76.6666666666667</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C7" s="1">
+        <v>81</v>
+      </c>
+      <c r="D7" s="1">
+        <v>73</v>
+      </c>
+      <c r="E7" s="1">
+        <v>79</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="0"/>
+        <v>233</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="1"/>
+        <v>77.6666666666667</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="1">
+        <v>82</v>
+      </c>
+      <c r="D8" s="1">
+        <v>77</v>
+      </c>
+      <c r="E8" s="1">
+        <v>80</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>239</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="1"/>
+        <v>79.6666666666667</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C9" s="1">
+        <v>83</v>
+      </c>
+      <c r="D9" s="1">
+        <v>78</v>
+      </c>
+      <c r="E9" s="1">
+        <v>81</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="0"/>
+        <v>242</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="1"/>
+        <v>80.6666666666667</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" s="1">
+        <v>84</v>
+      </c>
+      <c r="D10" s="1">
+        <v>79</v>
+      </c>
+      <c r="E10" s="1">
+        <v>77</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C11" s="1">
+        <v>85</v>
+      </c>
+      <c r="D11" s="1">
+        <v>80</v>
+      </c>
+      <c r="E11" s="1">
+        <v>78</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="0"/>
+        <v>243</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7">
+      <c r="B12" t="s">
+        <v>145</v>
+      </c>
+      <c r="C12">
+        <f>AVERAGE(C2:C11)</f>
+        <v>72.1</v>
+      </c>
+      <c r="D12">
+        <f>AVERAGE(D2:D11)</f>
+        <v>73.7</v>
+      </c>
+      <c r="E12">
+        <f>AVERAGE(E2:E11)</f>
+        <v>82.3</v>
+      </c>
+      <c r="F12">
+        <f>AVERAGE(F2:F11)</f>
+        <v>228.1</v>
+      </c>
+      <c r="G12">
+        <f>AVERAGE(G2:G11)</f>
+        <v>76.0333333333333</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="13.8" outlineLevelCol="5"/>
+  <cols>
+    <col min="2" max="2" width="15.6666666666667" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="1">
+        <v>55</v>
+      </c>
+      <c r="D2" s="1">
+        <v>68</v>
+      </c>
+      <c r="E2" s="1">
+        <v>90</v>
+      </c>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C3" s="1">
+        <v>56</v>
+      </c>
+      <c r="D3" s="1">
+        <v>69</v>
+      </c>
+      <c r="E3" s="1">
+        <v>91</v>
+      </c>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="1">
+        <v>57</v>
+      </c>
+      <c r="D4" s="1">
+        <v>70</v>
+      </c>
+      <c r="E4" s="1">
+        <v>92</v>
+      </c>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="1">
+        <v>58</v>
+      </c>
+      <c r="D5" s="1">
+        <v>71</v>
+      </c>
+      <c r="E5" s="1">
+        <v>77</v>
+      </c>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" s="1">
+        <v>80</v>
+      </c>
+      <c r="D6" s="1">
+        <v>72</v>
+      </c>
+      <c r="E6" s="1">
+        <v>78</v>
+      </c>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C7" s="1">
+        <v>81</v>
+      </c>
+      <c r="D7" s="1">
+        <v>73</v>
+      </c>
+      <c r="E7" s="1">
+        <v>79</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="1">
+        <v>82</v>
+      </c>
+      <c r="D8" s="1">
+        <v>77</v>
+      </c>
+      <c r="E8" s="1">
+        <v>80</v>
+      </c>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C9" s="1">
+        <v>83</v>
+      </c>
+      <c r="D9" s="1">
+        <v>78</v>
+      </c>
+      <c r="E9" s="1">
+        <v>81</v>
+      </c>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" s="1">
+        <v>84</v>
+      </c>
+      <c r="D10" s="1">
+        <v>79</v>
+      </c>
+      <c r="E10" s="1">
+        <v>77</v>
+      </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C11" s="1">
+        <v>85</v>
+      </c>
+      <c r="D11" s="1">
+        <v>80</v>
+      </c>
+      <c r="E11" s="1">
+        <v>78</v>
+      </c>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" s="2">
+        <v>55</v>
+      </c>
+      <c r="D12" s="2">
+        <v>68</v>
+      </c>
+      <c r="E12" s="2">
+        <v>90</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C13" s="2">
+        <v>56</v>
+      </c>
+      <c r="D13" s="2">
+        <v>69</v>
+      </c>
+      <c r="E13" s="2">
+        <v>91</v>
+      </c>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" s="2">
+        <v>57</v>
+      </c>
+      <c r="D14" s="2">
+        <v>70</v>
+      </c>
+      <c r="E14" s="2">
+        <v>92</v>
+      </c>
+      <c r="F14" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="A1:C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="13.8" outlineLevelCol="2"/>
+  <cols>
+    <col min="2" max="2" width="13.1111111111111" customWidth="1"/>
+    <col min="3" max="3" width="20.7777777777778" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2">
+        <v>1000</v>
+      </c>
+      <c r="C2">
+        <v>3999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3">
+        <v>2000</v>
+      </c>
+      <c r="C3">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B4">
+        <v>2001</v>
+      </c>
+      <c r="C4">
+        <v>4001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B5">
+        <v>2002</v>
+      </c>
+      <c r="C5">
+        <v>4002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>153</v>
+      </c>
+      <c r="B6">
+        <v>2003</v>
+      </c>
+      <c r="C6">
+        <v>4003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B7">
+        <v>2004</v>
+      </c>
+      <c r="C7">
+        <v>4004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B8">
+        <v>2005</v>
+      </c>
+      <c r="C8">
+        <v>4005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>156</v>
+      </c>
+      <c r="B9">
+        <v>2006</v>
+      </c>
+      <c r="C9">
+        <v>4006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>157</v>
+      </c>
+      <c r="B10">
+        <v>2007</v>
+      </c>
+      <c r="C10">
+        <v>4007</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11">
+        <v>2008</v>
+      </c>
+      <c r="C11">
+        <v>4008</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12">
+        <v>2009</v>
+      </c>
+      <c r="C12">
+        <v>4009</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13">
+        <v>2010</v>
+      </c>
+      <c r="C13">
+        <v>4010</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
@@ -8639,50 +9655,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="5">
         <v>12318</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="5">
         <v>17664</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="5">
         <v>19483</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="5">
         <v>33947</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="5">
         <v>59736</v>
       </c>
     </row>
@@ -8695,42 +9711,42 @@
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="5">
         <v>81304</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="5">
         <v>141651</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="5">
         <v>185107</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="5">
         <v>200312</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="5">
         <v>216932</v>
       </c>
     </row>
@@ -8738,7 +9754,7 @@
       <c r="P16"/>
     </row>
     <row r="19" ht="27.6" spans="4:4">
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="9" t="s">
         <v>19</v>
       </c>
     </row>
@@ -8766,32 +9782,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4">
+      <c r="B1" s="6">
         <v>2016</v>
       </c>
-      <c r="C1" s="4">
+      <c r="C1" s="6">
         <v>2017</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="5">
         <v>216932</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="5">
         <v>230711</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="5">
         <v>200312</v>
       </c>
       <c r="C3">
@@ -8799,65 +9815,65 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="5">
         <v>141651</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="5">
         <v>167180</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="5">
         <v>81318</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="5">
         <v>87577</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="5">
         <v>81304</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="5">
         <v>83046</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="5">
         <v>75385</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="5">
         <v>76838</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="5">
         <v>59736</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="5">
         <v>61506</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="5">
         <v>40877</v>
       </c>
       <c r="C9">
@@ -8865,68 +9881,68 @@
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="5">
         <v>21160</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="5">
         <v>21913</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="5">
         <v>26675</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="5">
         <v>21131</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="5">
         <v>19483</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="5">
         <v>17993</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="5">
         <v>17664</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="5">
         <v>17561</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="5">
         <v>15077</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="5">
         <v>15306</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="5">
         <v>12318</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="5">
         <v>12602</v>
       </c>
     </row>
@@ -8939,10 +9955,10 @@
       </c>
     </row>
     <row r="21" ht="110.4" spans="5:6">
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F21" s="8" t="s">
         <v>23</v>
       </c>
     </row>
@@ -8994,16 +10010,16 @@
       </c>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="3">
+      <c r="A2" s="5">
         <v>18</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="5">
         <v>11.22</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>28</v>
       </c>
       <c r="J2">
@@ -9020,16 +10036,16 @@
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="3">
+      <c r="A3" s="5">
         <v>15</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="5">
         <v>10.31</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="5" t="s">
         <v>28</v>
       </c>
       <c r="J3">
@@ -9072,16 +10088,16 @@
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="3">
+      <c r="A5" s="5">
         <v>9</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="5">
         <v>8.98</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="5" t="s">
         <v>28</v>
       </c>
       <c r="J5">
@@ -9098,16 +10114,16 @@
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="3">
+      <c r="A6" s="5">
         <v>6</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="5">
         <v>7.34</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="5" t="s">
         <v>28</v>
       </c>
       <c r="J6">
@@ -9124,16 +10140,16 @@
       </c>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="3">
+      <c r="A7" s="5">
         <v>12</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="5">
         <v>7.29</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="5" t="s">
         <v>28</v>
       </c>
       <c r="J7">
@@ -9150,16 +10166,16 @@
       </c>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="3">
+      <c r="A8" s="5">
         <v>2</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="5">
         <v>11.99</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="5" t="s">
         <v>30</v>
       </c>
       <c r="J8">
@@ -9176,16 +10192,16 @@
       </c>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" s="3">
+      <c r="A9" s="5">
         <v>17</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="5">
         <v>11.95</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="5" t="s">
         <v>30</v>
       </c>
       <c r="J9">
@@ -9202,16 +10218,16 @@
       </c>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="3">
+      <c r="A10" s="5">
         <v>8</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="5">
         <v>11.14</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="5" t="s">
         <v>30</v>
       </c>
       <c r="J10">
@@ -9228,16 +10244,16 @@
       </c>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="3">
+      <c r="A11" s="5">
         <v>4</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="5">
         <v>11.08</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="5" t="s">
         <v>30</v>
       </c>
       <c r="J11">
@@ -9254,16 +10270,16 @@
       </c>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="3">
+      <c r="A12" s="5">
         <v>7</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="5">
         <v>10.97</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="5" t="s">
         <v>30</v>
       </c>
       <c r="J12">
@@ -9280,16 +10296,16 @@
       </c>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="3">
+      <c r="A13" s="5">
         <v>19</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="5">
         <v>10.95</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="5" t="s">
         <v>30</v>
       </c>
       <c r="J13">
@@ -9306,16 +10322,16 @@
       </c>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="3">
+      <c r="A14" s="5">
         <v>16</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="5">
         <v>10.26</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="5" t="s">
         <v>30</v>
       </c>
       <c r="J14">
@@ -9332,16 +10348,16 @@
       </c>
     </row>
     <row r="15" spans="1:13">
-      <c r="A15" s="3">
+      <c r="A15" s="5">
         <v>1</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="5">
         <v>9.82</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="5" t="s">
         <v>30</v>
       </c>
       <c r="J15">
@@ -9358,16 +10374,16 @@
       </c>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="3">
+      <c r="A16" s="5">
         <v>10</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="5">
         <v>9.18</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="5" t="s">
         <v>30</v>
       </c>
       <c r="J16">
@@ -9384,16 +10400,16 @@
       </c>
     </row>
     <row r="17" spans="1:13">
-      <c r="A17" s="3">
+      <c r="A17" s="5">
         <v>14</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="5">
         <v>9.16</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="5" t="s">
         <v>30</v>
       </c>
       <c r="J17">
@@ -9410,16 +10426,16 @@
       </c>
     </row>
     <row r="18" spans="1:13">
-      <c r="A18" s="3">
+      <c r="A18" s="5">
         <v>20</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="5">
         <v>8.82</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="5" t="s">
         <v>30</v>
       </c>
       <c r="J18">
@@ -9436,16 +10452,16 @@
       </c>
     </row>
     <row r="19" spans="1:13">
-      <c r="A19" s="3">
+      <c r="A19" s="5">
         <v>13</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="5">
         <v>8.36</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="5" t="s">
         <v>30</v>
       </c>
       <c r="J19">
@@ -9462,16 +10478,16 @@
       </c>
     </row>
     <row r="20" spans="1:13">
-      <c r="A20" s="3">
+      <c r="A20" s="5">
         <v>11</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="5">
         <v>8.31</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="5" t="s">
         <v>30</v>
       </c>
       <c r="J20">
@@ -9488,16 +10504,16 @@
       </c>
     </row>
     <row r="21" spans="1:13">
-      <c r="A21" s="3">
+      <c r="A21" s="5">
         <v>5</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="5">
         <v>7.75</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="5" t="s">
         <v>30</v>
       </c>
       <c r="J21">
@@ -10147,22 +11163,22 @@
       </c>
     </row>
     <row r="2" spans="1:21">
-      <c r="A2" s="3">
+      <c r="A2" s="5">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="5">
         <v>11</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="5">
         <v>14</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="5">
         <v>17</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="5">
         <f t="shared" ref="F2:F11" si="0">C2+D2+E2</f>
         <v>42</v>
       </c>
@@ -10183,22 +11199,22 @@
       </c>
     </row>
     <row r="3" spans="1:21">
-      <c r="A3" s="3">
+      <c r="A3" s="5">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="5">
         <v>12</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="5">
         <v>10</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="5">
         <v>17</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="5">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
@@ -10219,22 +11235,22 @@
       </c>
     </row>
     <row r="4" spans="1:21">
-      <c r="A4" s="3">
+      <c r="A4" s="5">
         <v>8</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="5">
         <v>9</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="5">
         <v>12</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="5">
         <v>16</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="5">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
@@ -10255,22 +11271,22 @@
       </c>
     </row>
     <row r="5" spans="1:21">
-      <c r="A5" s="3">
+      <c r="A5" s="5">
         <v>9</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="5">
         <v>11</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="5">
         <v>11</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="5">
         <v>15</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="5">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
@@ -10291,22 +11307,22 @@
       </c>
     </row>
     <row r="6" spans="1:21">
-      <c r="A6" s="3">
+      <c r="A6" s="5">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="5">
         <v>8</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="5">
         <v>14</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="5">
         <v>13</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="5">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
@@ -10327,22 +11343,22 @@
       </c>
     </row>
     <row r="7" spans="1:21">
-      <c r="A7" s="3">
+      <c r="A7" s="5">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="5">
         <v>8</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="5">
         <v>11</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="5">
         <v>16</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="5">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
@@ -10363,22 +11379,22 @@
       </c>
     </row>
     <row r="8" spans="1:21">
-      <c r="A8" s="3">
+      <c r="A8" s="5">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="5">
         <v>11</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="5">
         <v>9</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="5">
         <v>14</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="5">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
@@ -10399,22 +11415,22 @@
       </c>
     </row>
     <row r="9" spans="1:21">
-      <c r="A9" s="3">
+      <c r="A9" s="5">
         <v>10</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="5">
         <v>9</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="5">
         <v>15</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="5">
         <v>10</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="5">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
@@ -10435,22 +11451,22 @@
       </c>
     </row>
     <row r="10" spans="1:21">
-      <c r="A10" s="3">
+      <c r="A10" s="5">
         <v>2</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="5">
         <v>10</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="5">
         <v>13</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="5">
         <v>10</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="5">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
@@ -10471,22 +11487,22 @@
       </c>
     </row>
     <row r="11" spans="1:21">
-      <c r="A11" s="3">
+      <c r="A11" s="5">
         <v>1</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="5">
         <v>7</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="5">
         <v>15</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="5">
         <v>10</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="5">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
@@ -10531,10 +11547,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C1" t="s">
@@ -10542,10 +11558,10 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="2">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>87</v>
       </c>
       <c r="C2">
@@ -10554,10 +11570,10 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="2">
+      <c r="A3" s="3">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>88</v>
       </c>
       <c r="C3">
@@ -10566,10 +11582,10 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="2">
+      <c r="A4" s="3">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>89</v>
       </c>
       <c r="C4">
@@ -10578,10 +11594,10 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="2">
+      <c r="A5" s="3">
         <v>7</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>90</v>
       </c>
       <c r="C5">
@@ -10590,10 +11606,10 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="2">
+      <c r="A6" s="3">
         <v>9</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>91</v>
       </c>
       <c r="C6">
@@ -10602,10 +11618,10 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="2">
+      <c r="A7" s="3">
         <v>11</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>92</v>
       </c>
       <c r="C7">
@@ -10614,10 +11630,10 @@
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="2">
+      <c r="A8" s="3">
         <v>13</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>93</v>
       </c>
       <c r="C8">
@@ -10626,10 +11642,10 @@
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="2">
+      <c r="A9" s="3">
         <v>15</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>94</v>
       </c>
       <c r="C9">
@@ -10638,10 +11654,10 @@
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="2">
+      <c r="A10" s="3">
         <v>17</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>95</v>
       </c>
       <c r="C10">
@@ -10650,10 +11666,10 @@
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="2">
+      <c r="A11" s="3">
         <v>19</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>96</v>
       </c>
       <c r="C11">
@@ -10662,10 +11678,10 @@
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="2">
+      <c r="A12" s="3">
         <v>21</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>97</v>
       </c>
       <c r="C12">
@@ -10674,10 +11690,10 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="2">
+      <c r="A13" s="3">
         <v>23</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>98</v>
       </c>
       <c r="C13">
@@ -10686,10 +11702,10 @@
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="2">
+      <c r="A14" s="3">
         <v>25</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>99</v>
       </c>
       <c r="C14">
@@ -10698,10 +11714,10 @@
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="2">
+      <c r="A15" s="3">
         <v>27</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>100</v>
       </c>
       <c r="C15">
@@ -10710,10 +11726,10 @@
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="2">
+      <c r="A16" s="3">
         <v>29</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>101</v>
       </c>
       <c r="C16">

</xml_diff>